<commit_message>
existing client populate done?
</commit_message>
<xml_diff>
--- a/src/mongodb/xls/patients.xlsx
+++ b/src/mongodb/xls/patients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyoungpark/Documents/kh_proj/mongodb/xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyoungpark/Documents/kh_proj/src/mongodb/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,9 +74,6 @@
     <t>1992-09-17</t>
   </si>
   <si>
-    <t>질병_1</t>
-  </si>
-  <si>
     <t>2017-03-06</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>1990-02-21</t>
   </si>
   <si>
-    <t>질병_2, 질병_4</t>
-  </si>
-  <si>
     <t>2015-12-13</t>
   </si>
   <si>
@@ -113,18 +107,12 @@
     <t>1984-08-20</t>
   </si>
   <si>
-    <t>질병_1, 질병_3</t>
-  </si>
-  <si>
     <t>2017-04-17</t>
   </si>
   <si>
     <t>1988-08-10</t>
   </si>
   <si>
-    <t>질병_7</t>
-  </si>
-  <si>
     <t>2016-01-01</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>1945-12-30</t>
   </si>
   <si>
-    <t>질병_3, 질병_8</t>
-  </si>
-  <si>
     <t>2016-01-04</t>
   </si>
   <si>
@@ -146,9 +131,6 @@
     <t>2010-01-30</t>
   </si>
   <si>
-    <t>질병_2, 질병_3</t>
-  </si>
-  <si>
     <t>2017-02-02</t>
   </si>
   <si>
@@ -174,6 +156,24 @@
   </si>
   <si>
     <t>(식품명_6:3), (식품명_10:1)</t>
+  </si>
+  <si>
+    <t>질병명_1</t>
+  </si>
+  <si>
+    <t>질병명_2,질병명_4</t>
+  </si>
+  <si>
+    <t>질병명_7</t>
+  </si>
+  <si>
+    <t>질병명_1,질병명_3</t>
+  </si>
+  <si>
+    <t>질병명_3,질병명_8</t>
+  </si>
+  <si>
+    <t>질병명_2,질병명_3</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -595,13 +595,13 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="P1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="11"/>
     </row>
@@ -628,10 +628,10 @@
         <v>주소_1</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="I2" s="6">
         <v>2</v>
@@ -643,13 +643,13 @@
         <v>70</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -665,20 +665,20 @@
         <v>이름_2</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="5" t="str">
         <f t="shared" si="1"/>
         <v>주소_2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="6">
         <v>3</v>
@@ -690,16 +690,16 @@
         <v>54</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -715,20 +715,20 @@
         <v>이름_3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5" t="str">
         <f t="shared" si="1"/>
         <v>주소_3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="6">
         <v>1</v>
@@ -740,16 +740,16 @@
         <v>45</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -765,20 +765,20 @@
         <v>이름_4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="str">
         <f t="shared" si="1"/>
         <v>주소_4</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I5" s="6">
         <v>1</v>
@@ -790,10 +790,10 @@
         <v>60</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N5" s="6"/>
     </row>
@@ -813,17 +813,17 @@
         <v>13</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="str">
         <f t="shared" si="1"/>
         <v>주소_5</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I6" s="6">
         <v>3</v>
@@ -835,19 +835,19 @@
         <v>100</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -866,17 +866,17 @@
         <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F7" s="5" t="str">
         <f t="shared" si="1"/>
         <v>주소_6</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I7" s="6">
         <v>2</v>
@@ -888,16 +888,16 @@
         <v>49</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -913,20 +913,20 @@
         <v>이름_7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5" t="str">
         <f t="shared" si="1"/>
         <v>주소_7</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I8" s="6">
         <v>1</v>
@@ -938,13 +938,13 @@
         <v>45</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>